<commit_message>
first full build of image POAM exporter
</commit_message>
<xml_diff>
--- a/reporting/POAM_Export_Sample.xlsx
+++ b/reporting/POAM_Export_Sample.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
   <workbookPr codeName="ThisWorkbook" hidePivotFieldList="1" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonathanspigler/Documents/NAVSEA-NSWCCD/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonathanspigler/projects/c-ato/reporting/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F6BA7B13-93FC-E34C-9B9E-4E1CE51F7225}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EB73E9B-9FD5-DF44-ACB6-A2BD29149126}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="16120" tabRatio="527" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1749" uniqueCount="409">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1683" uniqueCount="387">
   <si>
     <t>MAC I / CL</t>
   </si>
@@ -977,9 +977,6 @@
     <t>DoD</t>
   </si>
   <si>
-    <t>DoD, John Smith, 7033775472, smith_john@email.com</t>
-  </si>
-  <si>
     <t>III</t>
   </si>
   <si>
@@ -1025,12 +1022,6 @@
     <t>john.smith@mail.mil</t>
   </si>
   <si>
-    <t>SV-18394r2_rule</t>
-  </si>
-  <si>
-    <t>SV-40098r2_rule</t>
-  </si>
-  <si>
     <t>Security Checks</t>
   </si>
   <si>
@@ -1088,67 +1079,10 @@
     <t>Very High</t>
   </si>
   <si>
-    <t>Summary of the recommended actions that will further address/reduce the risk of this vulnerability.</t>
-  </si>
-  <si>
-    <t>Narrative description of how this vulnerability was discovered (annual review, automated scan, etc.)</t>
-  </si>
-  <si>
-    <t>Resources required to correct the identified vulnerability.</t>
-  </si>
-  <si>
     <t>IS Enclave</t>
   </si>
   <si>
     <t>2/20/2018</t>
-  </si>
-  <si>
-    <t>Description that explains the identified vulnerability and any other pertinent information.</t>
-  </si>
-  <si>
-    <t>AC-1</t>
-  </si>
-  <si>
-    <t>Implement Procedure A 10/25/2018</t>
-  </si>
-  <si>
-    <t>Description of any relevant information not captured by the other fields.</t>
-  </si>
-  <si>
-    <t>Implement Procedure B 10/31/2018</t>
-  </si>
-  <si>
-    <t>Implement Procedure C 11/5/2018</t>
-  </si>
-  <si>
-    <t>SA-1.4</t>
-  </si>
-  <si>
-    <t>Example Program Management Office</t>
-  </si>
-  <si>
-    <t>Description of Milestone 10/17/2018</t>
-  </si>
-  <si>
-    <t>Updated Milestone Description 10/22/2018</t>
-  </si>
-  <si>
-    <t>Completed 11/13/2018</t>
-  </si>
-  <si>
-    <t>Description of the mitigations in place (if any) to counter this vulnerability.</t>
-  </si>
-  <si>
-    <t>Description of the predisposing conditions (if any).</t>
-  </si>
-  <si>
-    <t>Description of the identified theat(s).</t>
-  </si>
-  <si>
-    <t>Identify affected devices.</t>
-  </si>
-  <si>
-    <t>Description of magnitude of potential harm from the exploitation of this vulnerability.</t>
   </si>
   <si>
     <t>***** UNCLASSIFIED//FOR OFFICIAL USE ONLY *****</t>
@@ -1992,6 +1926,7 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -2748,11 +2683,8 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2765,6 +2697,30 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="6" fontId="8" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -2795,27 +2751,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="6" fontId="8" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="13" borderId="23" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -3514,13 +3449,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="B2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.15">
@@ -3531,23 +3466,23 @@
         <v>26</v>
       </c>
       <c r="C3" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B4" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="C4" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="B5" t="s">
         <v>17</v>
@@ -3555,10 +3490,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
+        <v>341</v>
+      </c>
+      <c r="B6" t="s">
         <v>344</v>
-      </c>
-      <c r="B6" t="s">
-        <v>347</v>
       </c>
     </row>
   </sheetData>
@@ -8967,8 +8902,8 @@
   </sheetPr>
   <dimension ref="A1:FU51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="T7" sqref="T7"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.15"/>
@@ -8995,63 +8930,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:177" s="18" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="76" t="s">
-        <v>369</v>
-      </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
-      <c r="D1" s="77"/>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
-      <c r="G1" s="77"/>
-      <c r="H1" s="77"/>
-      <c r="I1" s="77"/>
-      <c r="J1" s="77"/>
-      <c r="K1" s="77"/>
-      <c r="L1" s="77"/>
-      <c r="M1" s="77"/>
-      <c r="N1" s="77"/>
-      <c r="O1" s="77"/>
-      <c r="P1" s="77"/>
-      <c r="Q1" s="77"/>
-      <c r="R1" s="77"/>
-      <c r="S1" s="77"/>
-      <c r="T1" s="77"/>
-      <c r="U1" s="77"/>
-      <c r="V1" s="77"/>
-      <c r="W1" s="77"/>
-      <c r="X1" s="77"/>
-      <c r="Y1" s="77"/>
+      <c r="A1" s="87" t="s">
+        <v>347</v>
+      </c>
+      <c r="B1" s="88"/>
+      <c r="C1" s="88"/>
+      <c r="D1" s="88"/>
+      <c r="E1" s="88"/>
+      <c r="F1" s="88"/>
+      <c r="G1" s="88"/>
+      <c r="H1" s="88"/>
+      <c r="I1" s="88"/>
+      <c r="J1" s="88"/>
+      <c r="K1" s="88"/>
+      <c r="L1" s="88"/>
+      <c r="M1" s="88"/>
+      <c r="N1" s="88"/>
+      <c r="O1" s="88"/>
+      <c r="P1" s="88"/>
+      <c r="Q1" s="88"/>
+      <c r="R1" s="88"/>
+      <c r="S1" s="88"/>
+      <c r="T1" s="88"/>
+      <c r="U1" s="88"/>
+      <c r="V1" s="88"/>
+      <c r="W1" s="88"/>
+      <c r="X1" s="88"/>
+      <c r="Y1" s="88"/>
       <c r="Z1" s="44"/>
     </row>
     <row r="2" spans="1:177" s="18" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="78" t="s">
+      <c r="A2" s="77" t="s">
         <v>299</v>
       </c>
-      <c r="B2" s="78"/>
-      <c r="C2" s="79" t="s">
-        <v>352</v>
-      </c>
-      <c r="D2" s="80"/>
-      <c r="E2" s="80"/>
-      <c r="F2" s="80"/>
-      <c r="G2" s="80"/>
-      <c r="H2" s="81"/>
-      <c r="I2" s="86" t="s">
-        <v>318</v>
-      </c>
-      <c r="J2" s="88" t="s">
-        <v>351</v>
-      </c>
-      <c r="K2" s="89"/>
-      <c r="L2" s="78" t="s">
+      <c r="B2" s="77"/>
+      <c r="C2" s="78" t="s">
+        <v>346</v>
+      </c>
+      <c r="D2" s="79"/>
+      <c r="E2" s="79"/>
+      <c r="F2" s="79"/>
+      <c r="G2" s="79"/>
+      <c r="H2" s="80"/>
+      <c r="I2" s="93" t="s">
+        <v>317</v>
+      </c>
+      <c r="J2" s="95" t="s">
+        <v>345</v>
+      </c>
+      <c r="K2" s="96"/>
+      <c r="L2" s="77" t="s">
         <v>294</v>
       </c>
-      <c r="M2" s="85">
+      <c r="M2" s="92">
         <v>54324</v>
       </c>
-      <c r="N2" s="85"/>
-      <c r="O2" s="85"/>
+      <c r="N2" s="92"/>
+      <c r="O2" s="92"/>
       <c r="P2" s="32"/>
       <c r="Q2" s="28"/>
       <c r="R2" s="28"/>
@@ -9064,25 +8999,25 @@
       <c r="Y2" s="29"/>
     </row>
     <row r="3" spans="1:177" s="18" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="78" t="s">
+      <c r="A3" s="77" t="s">
         <v>300</v>
       </c>
-      <c r="B3" s="78"/>
-      <c r="C3" s="79" t="s">
+      <c r="B3" s="77"/>
+      <c r="C3" s="78" t="s">
         <v>309</v>
       </c>
-      <c r="D3" s="80"/>
-      <c r="E3" s="80"/>
-      <c r="F3" s="80"/>
-      <c r="G3" s="80"/>
-      <c r="H3" s="81"/>
-      <c r="I3" s="87"/>
-      <c r="J3" s="90"/>
-      <c r="K3" s="91"/>
-      <c r="L3" s="78"/>
-      <c r="M3" s="85"/>
-      <c r="N3" s="85"/>
-      <c r="O3" s="85"/>
+      <c r="D3" s="79"/>
+      <c r="E3" s="79"/>
+      <c r="F3" s="79"/>
+      <c r="G3" s="79"/>
+      <c r="H3" s="80"/>
+      <c r="I3" s="94"/>
+      <c r="J3" s="97"/>
+      <c r="K3" s="98"/>
+      <c r="L3" s="77"/>
+      <c r="M3" s="92"/>
+      <c r="N3" s="92"/>
+      <c r="O3" s="92"/>
       <c r="P3" s="33"/>
       <c r="Q3" s="26"/>
       <c r="R3" s="26"/>
@@ -9095,29 +9030,29 @@
       <c r="Y3" s="30"/>
     </row>
     <row r="4" spans="1:177" s="18" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="78" t="s">
-        <v>317</v>
-      </c>
-      <c r="B4" s="78"/>
-      <c r="C4" s="79" t="s">
+      <c r="A4" s="77" t="s">
+        <v>316</v>
+      </c>
+      <c r="B4" s="77"/>
+      <c r="C4" s="78" t="s">
         <v>310</v>
       </c>
-      <c r="D4" s="80"/>
-      <c r="E4" s="80"/>
-      <c r="F4" s="80"/>
-      <c r="G4" s="80"/>
-      <c r="H4" s="81"/>
+      <c r="D4" s="79"/>
+      <c r="E4" s="79"/>
+      <c r="F4" s="79"/>
+      <c r="G4" s="79"/>
+      <c r="H4" s="80"/>
       <c r="I4" s="45" t="s">
-        <v>320</v>
-      </c>
-      <c r="J4" s="82" t="s">
+        <v>319</v>
+      </c>
+      <c r="J4" s="89" t="s">
         <v>309</v>
       </c>
-      <c r="K4" s="83"/>
-      <c r="L4" s="78"/>
-      <c r="M4" s="78"/>
-      <c r="N4" s="78"/>
-      <c r="O4" s="84"/>
+      <c r="K4" s="90"/>
+      <c r="L4" s="77"/>
+      <c r="M4" s="77"/>
+      <c r="N4" s="77"/>
+      <c r="O4" s="91"/>
       <c r="P4" s="33"/>
       <c r="Q4" s="26"/>
       <c r="R4" s="26"/>
@@ -9130,33 +9065,33 @@
       <c r="Y4" s="30"/>
     </row>
     <row r="5" spans="1:177" s="18" customFormat="1" ht="17" x14ac:dyDescent="0.15">
-      <c r="A5" s="78" t="s">
+      <c r="A5" s="77" t="s">
         <v>295</v>
       </c>
-      <c r="B5" s="78"/>
-      <c r="C5" s="79" t="s">
+      <c r="B5" s="77"/>
+      <c r="C5" s="78" t="s">
         <v>308</v>
       </c>
-      <c r="D5" s="80"/>
-      <c r="E5" s="80"/>
-      <c r="F5" s="80"/>
-      <c r="G5" s="80"/>
-      <c r="H5" s="81"/>
+      <c r="D5" s="79"/>
+      <c r="E5" s="79"/>
+      <c r="F5" s="79"/>
+      <c r="G5" s="79"/>
+      <c r="H5" s="80"/>
       <c r="I5" s="10" t="s">
-        <v>321</v>
-      </c>
-      <c r="J5" s="93" t="s">
-        <v>325</v>
-      </c>
-      <c r="K5" s="94"/>
+        <v>320</v>
+      </c>
+      <c r="J5" s="81" t="s">
+        <v>324</v>
+      </c>
+      <c r="K5" s="82"/>
       <c r="L5" s="11" t="s">
         <v>296</v>
       </c>
-      <c r="M5" s="95">
+      <c r="M5" s="83">
         <v>10000</v>
       </c>
-      <c r="N5" s="94"/>
-      <c r="O5" s="94"/>
+      <c r="N5" s="82"/>
+      <c r="O5" s="82"/>
       <c r="P5" s="33"/>
       <c r="Q5" s="26"/>
       <c r="R5" s="26"/>
@@ -9169,29 +9104,29 @@
       <c r="Y5" s="30"/>
     </row>
     <row r="6" spans="1:177" s="18" customFormat="1" ht="17" x14ac:dyDescent="0.15">
-      <c r="A6" s="78" t="s">
+      <c r="A6" s="77" t="s">
         <v>297</v>
       </c>
-      <c r="B6" s="78"/>
-      <c r="C6" s="79">
+      <c r="B6" s="77"/>
+      <c r="C6" s="78">
         <v>5050</v>
       </c>
-      <c r="D6" s="80"/>
-      <c r="E6" s="80"/>
-      <c r="F6" s="80"/>
-      <c r="G6" s="80"/>
-      <c r="H6" s="81"/>
+      <c r="D6" s="79"/>
+      <c r="E6" s="79"/>
+      <c r="F6" s="79"/>
+      <c r="G6" s="79"/>
+      <c r="H6" s="80"/>
       <c r="I6" s="10" t="s">
-        <v>322</v>
-      </c>
-      <c r="J6" s="96" t="s">
-        <v>326</v>
-      </c>
-      <c r="K6" s="94"/>
-      <c r="L6" s="97"/>
-      <c r="M6" s="98"/>
-      <c r="N6" s="98"/>
-      <c r="O6" s="98"/>
+        <v>321</v>
+      </c>
+      <c r="J6" s="84" t="s">
+        <v>325</v>
+      </c>
+      <c r="K6" s="82"/>
+      <c r="L6" s="85"/>
+      <c r="M6" s="86"/>
+      <c r="N6" s="86"/>
+      <c r="O6" s="86"/>
       <c r="P6" s="34"/>
       <c r="Q6" s="27"/>
       <c r="R6" s="27"/>
@@ -9204,18 +9139,18 @@
       <c r="Y6" s="31"/>
     </row>
     <row r="7" spans="1:177" s="22" customFormat="1" ht="68" x14ac:dyDescent="0.15">
-      <c r="A7" s="92" t="s">
+      <c r="A7" s="76" t="s">
+        <v>314</v>
+      </c>
+      <c r="B7" s="76"/>
+      <c r="C7" s="46" t="s">
+        <v>313</v>
+      </c>
+      <c r="D7" s="46" t="s">
         <v>315</v>
       </c>
-      <c r="B7" s="92"/>
-      <c r="C7" s="46" t="s">
-        <v>314</v>
-      </c>
-      <c r="D7" s="46" t="s">
-        <v>316</v>
-      </c>
       <c r="E7" s="46" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="F7" s="46" t="s">
         <v>301</v>
@@ -9230,7 +9165,7 @@
         <v>306</v>
       </c>
       <c r="J7" s="46" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="K7" s="46" t="s">
         <v>303</v>
@@ -9239,119 +9174,73 @@
         <v>304</v>
       </c>
       <c r="M7" s="46" t="s">
+        <v>335</v>
+      </c>
+      <c r="N7" s="46" t="s">
+        <v>336</v>
+      </c>
+      <c r="O7" s="46" t="s">
+        <v>385</v>
+      </c>
+      <c r="P7" s="46" t="s">
+        <v>337</v>
+      </c>
+      <c r="Q7" s="46" t="s">
+        <v>328</v>
+      </c>
+      <c r="R7" s="46" t="s">
+        <v>329</v>
+      </c>
+      <c r="S7" s="46" t="s">
         <v>338</v>
       </c>
-      <c r="N7" s="46" t="s">
+      <c r="T7" s="46" t="s">
+        <v>330</v>
+      </c>
+      <c r="U7" s="46" t="s">
+        <v>331</v>
+      </c>
+      <c r="V7" s="46" t="s">
+        <v>332</v>
+      </c>
+      <c r="W7" s="46" t="s">
+        <v>333</v>
+      </c>
+      <c r="X7" s="46" t="s">
+        <v>334</v>
+      </c>
+      <c r="Y7" s="46" t="s">
         <v>339</v>
       </c>
-      <c r="O7" s="46" t="s">
-        <v>407</v>
-      </c>
-      <c r="P7" s="46" t="s">
-        <v>340</v>
-      </c>
-      <c r="Q7" s="46" t="s">
-        <v>331</v>
-      </c>
-      <c r="R7" s="46" t="s">
-        <v>332</v>
-      </c>
-      <c r="S7" s="46" t="s">
-        <v>341</v>
-      </c>
-      <c r="T7" s="46" t="s">
-        <v>333</v>
-      </c>
-      <c r="U7" s="46" t="s">
-        <v>334</v>
-      </c>
-      <c r="V7" s="46" t="s">
-        <v>335</v>
-      </c>
-      <c r="W7" s="46" t="s">
-        <v>336</v>
-      </c>
-      <c r="X7" s="46" t="s">
-        <v>337</v>
-      </c>
-      <c r="Y7" s="46" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="8" spans="1:177" s="18" customFormat="1" ht="102" x14ac:dyDescent="0.15">
+    </row>
+    <row r="8" spans="1:177" s="18" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A8" s="13"/>
-      <c r="B8" s="13" t="s">
-        <v>353</v>
-      </c>
-      <c r="C8" s="14" t="s">
-        <v>354</v>
-      </c>
-      <c r="D8" s="14" t="s">
-        <v>311</v>
-      </c>
-      <c r="E8" s="54" t="s">
-        <v>327</v>
-      </c>
-      <c r="F8" s="15" t="s">
-        <v>350</v>
-      </c>
-      <c r="G8" s="16">
-        <v>43427</v>
-      </c>
-      <c r="H8" s="14" t="s">
-        <v>355</v>
-      </c>
+      <c r="B8" s="13"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="54"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="14"/>
       <c r="I8" s="14"/>
-      <c r="J8" s="14" t="s">
-        <v>349</v>
-      </c>
-      <c r="K8" s="14" t="s">
-        <v>307</v>
-      </c>
-      <c r="L8" s="41" t="s">
-        <v>356</v>
-      </c>
-      <c r="M8" s="49" t="s">
-        <v>323</v>
-      </c>
-      <c r="N8" s="50" t="s">
-        <v>367</v>
-      </c>
-      <c r="O8" s="41" t="s">
-        <v>364</v>
-      </c>
-      <c r="P8" s="24" t="s">
-        <v>365</v>
-      </c>
-      <c r="Q8" s="49" t="s">
-        <v>17</v>
-      </c>
-      <c r="R8" s="49" t="s">
-        <v>17</v>
-      </c>
-      <c r="S8" s="24" t="s">
-        <v>366</v>
-      </c>
-      <c r="T8" s="49" t="s">
-        <v>17</v>
-      </c>
-      <c r="U8" s="49" t="s">
-        <v>17</v>
-      </c>
-      <c r="V8" s="24" t="s">
-        <v>368</v>
-      </c>
-      <c r="W8" s="48" t="s">
-        <v>17</v>
-      </c>
-      <c r="X8" s="48" t="s">
-        <v>348</v>
-      </c>
-      <c r="Y8" s="35" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="9" spans="1:177" s="18" customFormat="1" ht="34" x14ac:dyDescent="0.15">
+      <c r="J8" s="14"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="41"/>
+      <c r="M8" s="49"/>
+      <c r="N8" s="50"/>
+      <c r="O8" s="41"/>
+      <c r="P8" s="24"/>
+      <c r="Q8" s="49"/>
+      <c r="R8" s="49"/>
+      <c r="S8" s="24"/>
+      <c r="T8" s="49"/>
+      <c r="U8" s="49"/>
+      <c r="V8" s="24"/>
+      <c r="W8" s="48"/>
+      <c r="X8" s="48"/>
+      <c r="Y8" s="35"/>
+    </row>
+    <row r="9" spans="1:177" s="18" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A9" s="23"/>
       <c r="B9" s="13"/>
       <c r="C9" s="41"/>
@@ -9359,9 +9248,7 @@
       <c r="E9" s="13"/>
       <c r="F9" s="15"/>
       <c r="G9" s="51"/>
-      <c r="H9" s="14" t="s">
-        <v>357</v>
-      </c>
+      <c r="H9" s="14"/>
       <c r="I9" s="14"/>
       <c r="J9" s="14"/>
       <c r="K9" s="14"/>
@@ -9380,7 +9267,7 @@
       <c r="X9" s="48"/>
       <c r="Y9" s="35"/>
     </row>
-    <row r="10" spans="1:177" s="18" customFormat="1" ht="34" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:177" s="18" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A10" s="23"/>
       <c r="B10" s="13"/>
       <c r="C10" s="14"/>
@@ -9388,9 +9275,7 @@
       <c r="E10" s="13"/>
       <c r="F10" s="15"/>
       <c r="G10" s="16"/>
-      <c r="H10" s="14" t="s">
-        <v>358</v>
-      </c>
+      <c r="H10" s="14"/>
       <c r="I10" s="14"/>
       <c r="J10" s="14"/>
       <c r="K10" s="14"/>
@@ -9409,145 +9294,59 @@
       <c r="X10" s="48"/>
       <c r="Y10" s="35"/>
     </row>
-    <row r="11" spans="1:177" s="18" customFormat="1" ht="102" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:177" s="18" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A11" s="23"/>
-      <c r="B11" s="13" t="s">
-        <v>353</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>359</v>
-      </c>
-      <c r="D11" s="13" t="s">
-        <v>310</v>
-      </c>
-      <c r="E11" s="54" t="s">
-        <v>328</v>
-      </c>
-      <c r="F11" s="15" t="s">
-        <v>350</v>
-      </c>
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="54"/>
+      <c r="F11" s="15"/>
       <c r="G11" s="17"/>
       <c r="H11" s="13"/>
       <c r="I11" s="13"/>
-      <c r="J11" s="14" t="s">
-        <v>349</v>
-      </c>
-      <c r="K11" s="13" t="s">
-        <v>344</v>
-      </c>
-      <c r="L11" s="41" t="s">
-        <v>356</v>
-      </c>
-      <c r="M11" s="47" t="s">
-        <v>312</v>
-      </c>
-      <c r="N11" s="50" t="s">
-        <v>367</v>
-      </c>
-      <c r="O11" s="41" t="s">
-        <v>364</v>
-      </c>
-      <c r="P11" s="24" t="s">
-        <v>365</v>
-      </c>
-      <c r="Q11" s="47" t="s">
-        <v>319</v>
-      </c>
-      <c r="R11" s="47" t="s">
-        <v>26</v>
-      </c>
-      <c r="S11" s="24" t="s">
-        <v>366</v>
-      </c>
-      <c r="T11" s="53" t="s">
-        <v>319</v>
-      </c>
-      <c r="U11" s="48" t="s">
-        <v>346</v>
-      </c>
-      <c r="V11" s="24" t="s">
-        <v>368</v>
-      </c>
-      <c r="W11" s="52" t="s">
-        <v>26</v>
-      </c>
-      <c r="X11" s="48" t="s">
-        <v>348</v>
-      </c>
-      <c r="Y11" s="35" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="12" spans="1:177" s="18" customFormat="1" ht="102" x14ac:dyDescent="0.15">
+      <c r="J11" s="14"/>
+      <c r="K11" s="13"/>
+      <c r="L11" s="41"/>
+      <c r="M11" s="47"/>
+      <c r="N11" s="50"/>
+      <c r="O11" s="41"/>
+      <c r="P11" s="24"/>
+      <c r="Q11" s="47"/>
+      <c r="R11" s="47"/>
+      <c r="S11" s="24"/>
+      <c r="T11" s="53"/>
+      <c r="U11" s="48"/>
+      <c r="V11" s="24"/>
+      <c r="W11" s="52"/>
+      <c r="X11" s="48"/>
+      <c r="Y11" s="35"/>
+    </row>
+    <row r="12" spans="1:177" s="18" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A12" s="23"/>
-      <c r="B12" s="13" t="s">
-        <v>353</v>
-      </c>
+      <c r="B12" s="13"/>
       <c r="C12" s="37"/>
-      <c r="D12" s="13" t="s">
-        <v>360</v>
-      </c>
+      <c r="D12" s="13"/>
       <c r="E12" s="37"/>
-      <c r="F12" s="15" t="s">
-        <v>350</v>
-      </c>
-      <c r="G12" s="17">
-        <v>43398</v>
-      </c>
-      <c r="H12" s="13" t="s">
-        <v>361</v>
-      </c>
-      <c r="I12" s="13" t="s">
-        <v>362</v>
-      </c>
-      <c r="J12" s="14" t="s">
-        <v>349</v>
-      </c>
-      <c r="K12" s="13" t="s">
-        <v>363</v>
-      </c>
-      <c r="L12" s="41" t="s">
-        <v>356</v>
-      </c>
-      <c r="M12" s="47" t="s">
-        <v>312</v>
-      </c>
-      <c r="N12" s="50" t="s">
-        <v>367</v>
-      </c>
-      <c r="O12" s="41" t="s">
-        <v>364</v>
-      </c>
-      <c r="P12" s="24" t="s">
-        <v>365</v>
-      </c>
-      <c r="Q12" s="47" t="s">
-        <v>17</v>
-      </c>
-      <c r="R12" s="47" t="s">
-        <v>346</v>
-      </c>
-      <c r="S12" s="24" t="s">
-        <v>366</v>
-      </c>
-      <c r="T12" s="48" t="s">
-        <v>346</v>
-      </c>
-      <c r="U12" s="48" t="s">
-        <v>17</v>
-      </c>
-      <c r="V12" s="24" t="s">
-        <v>368</v>
-      </c>
-      <c r="W12" s="48" t="s">
-        <v>346</v>
-      </c>
-      <c r="X12" s="48" t="s">
-        <v>348</v>
-      </c>
-      <c r="Y12" s="35" t="s">
-        <v>26</v>
-      </c>
+      <c r="F12" s="15"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="13"/>
+      <c r="L12" s="41"/>
+      <c r="M12" s="47"/>
+      <c r="N12" s="50"/>
+      <c r="O12" s="41"/>
+      <c r="P12" s="24"/>
+      <c r="Q12" s="47"/>
+      <c r="R12" s="47"/>
+      <c r="S12" s="24"/>
+      <c r="T12" s="48"/>
+      <c r="U12" s="48"/>
+      <c r="V12" s="24"/>
+      <c r="W12" s="48"/>
+      <c r="X12" s="48"/>
+      <c r="Y12" s="35"/>
     </row>
     <row r="13" spans="1:177" s="18" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A13" s="23"/>
@@ -16533,15 +16332,6 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="22">
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:H5"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="M5:O5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:H6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="L6:O6"/>
     <mergeCell ref="A1:Y1"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="C4:H4"/>
@@ -16555,6 +16345,15 @@
     <mergeCell ref="I2:I3"/>
     <mergeCell ref="J2:K3"/>
     <mergeCell ref="L2:L3"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:H5"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="M5:O5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:H6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="L6:O6"/>
   </mergeCells>
   <conditionalFormatting sqref="T2:T6 T8:T1048576">
     <cfRule type="cellIs" dxfId="24" priority="24" operator="equal">
@@ -16665,10 +16464,9 @@
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="J6" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
-    <hyperlink ref="D11" r:id="rId2" display="smith_john@email.com" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup scale="53" fitToHeight="0" orientation="landscape" r:id="rId3"/>
+  <pageSetup scale="53" fitToHeight="0" orientation="landscape" r:id="rId2"/>
   <headerFooter alignWithMargins="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
@@ -16723,7 +16521,7 @@
     </row>
     <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A2" s="57" t="s">
-        <v>370</v>
+        <v>348</v>
       </c>
       <c r="B2" s="56"/>
       <c r="C2" s="56"/>
@@ -16733,7 +16531,7 @@
     </row>
     <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A3" s="57" t="s">
-        <v>371</v>
+        <v>349</v>
       </c>
       <c r="B3" s="56"/>
       <c r="C3" s="56"/>
@@ -16743,7 +16541,7 @@
     </row>
     <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A4" s="57" t="s">
-        <v>372</v>
+        <v>350</v>
       </c>
       <c r="B4" s="56"/>
       <c r="C4" s="56"/>
@@ -16753,7 +16551,7 @@
     </row>
     <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A5" s="57" t="s">
-        <v>373</v>
+        <v>351</v>
       </c>
       <c r="B5" s="56"/>
       <c r="C5" s="56"/>
@@ -16763,7 +16561,7 @@
     </row>
     <row r="6" spans="1:6" ht="32" x14ac:dyDescent="0.15">
       <c r="A6" s="57" t="s">
-        <v>374</v>
+        <v>352</v>
       </c>
       <c r="B6" s="56"/>
       <c r="C6" s="56"/>
@@ -16773,7 +16571,7 @@
     </row>
     <row r="7" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A7" s="57" t="s">
-        <v>375</v>
+        <v>353</v>
       </c>
       <c r="B7" s="56"/>
       <c r="C7" s="56"/>
@@ -16783,7 +16581,7 @@
     </row>
     <row r="8" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A8" s="57" t="s">
-        <v>376</v>
+        <v>354</v>
       </c>
       <c r="B8" s="56"/>
       <c r="C8" s="56"/>
@@ -16793,7 +16591,7 @@
     </row>
     <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A9" s="57" t="s">
-        <v>377</v>
+        <v>355</v>
       </c>
       <c r="B9" s="56"/>
       <c r="C9" s="56"/>
@@ -16803,7 +16601,7 @@
     </row>
     <row r="10" spans="1:6" ht="32" x14ac:dyDescent="0.15">
       <c r="A10" s="57" t="s">
-        <v>378</v>
+        <v>356</v>
       </c>
       <c r="B10" s="56"/>
       <c r="C10" s="56"/>
@@ -16813,7 +16611,7 @@
     </row>
     <row r="11" spans="1:6" ht="32" x14ac:dyDescent="0.15">
       <c r="A11" s="57" t="s">
-        <v>379</v>
+        <v>357</v>
       </c>
       <c r="B11" s="56"/>
       <c r="C11" s="56"/>
@@ -16823,7 +16621,7 @@
     </row>
     <row r="12" spans="1:6" ht="32" x14ac:dyDescent="0.15">
       <c r="A12" s="57" t="s">
-        <v>380</v>
+        <v>358</v>
       </c>
       <c r="B12" s="56"/>
       <c r="C12" s="56"/>
@@ -16833,7 +16631,7 @@
     </row>
     <row r="13" spans="1:6" ht="32" x14ac:dyDescent="0.15">
       <c r="A13" s="57" t="s">
-        <v>381</v>
+        <v>359</v>
       </c>
       <c r="B13" s="56"/>
       <c r="C13" s="56"/>
@@ -16843,7 +16641,7 @@
     </row>
     <row r="14" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A14" s="57" t="s">
-        <v>382</v>
+        <v>360</v>
       </c>
       <c r="B14" s="56"/>
       <c r="C14" s="56"/>
@@ -16853,7 +16651,7 @@
     </row>
     <row r="15" spans="1:6" ht="64" x14ac:dyDescent="0.15">
       <c r="A15" s="57" t="s">
-        <v>383</v>
+        <v>361</v>
       </c>
       <c r="B15" s="56"/>
       <c r="C15" s="56"/>
@@ -16863,62 +16661,62 @@
     </row>
     <row r="16" spans="1:6" ht="32" x14ac:dyDescent="0.15">
       <c r="A16" s="57" t="s">
-        <v>384</v>
+        <v>362</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="64" x14ac:dyDescent="0.15">
       <c r="A17" s="57" t="s">
-        <v>385</v>
+        <v>363</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="64" x14ac:dyDescent="0.15">
       <c r="A18" s="74" t="s">
-        <v>386</v>
+        <v>364</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="144" x14ac:dyDescent="0.15">
       <c r="A19" s="74" t="s">
-        <v>387</v>
+        <v>365</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="240" x14ac:dyDescent="0.15">
       <c r="A20" s="57" t="s">
-        <v>388</v>
+        <v>366</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="48" x14ac:dyDescent="0.15">
       <c r="A21" s="57" t="s">
-        <v>389</v>
+        <v>367</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="272" x14ac:dyDescent="0.15">
       <c r="A22" s="57" t="s">
-        <v>390</v>
+        <v>368</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="160" x14ac:dyDescent="0.15">
       <c r="A23" s="57" t="s">
-        <v>391</v>
+        <v>369</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="48" x14ac:dyDescent="0.15">
       <c r="A24" s="57" t="s">
-        <v>392</v>
+        <v>370</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="192" x14ac:dyDescent="0.15">
       <c r="A25" s="57" t="s">
-        <v>393</v>
+        <v>371</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="32" x14ac:dyDescent="0.15">
       <c r="A26" s="57" t="s">
-        <v>394</v>
+        <v>372</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="16" x14ac:dyDescent="0.15">
       <c r="A27" s="57" t="s">
-        <v>395</v>
+        <v>373</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="15" x14ac:dyDescent="0.15">
@@ -16926,22 +16724,22 @@
     </row>
     <row r="29" spans="1:8" ht="16" x14ac:dyDescent="0.15">
       <c r="A29" s="59" t="s">
-        <v>396</v>
+        <v>374</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="16" x14ac:dyDescent="0.15">
       <c r="A30" s="57" t="s">
-        <v>397</v>
+        <v>375</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="16" x14ac:dyDescent="0.15">
       <c r="A31" s="57" t="s">
-        <v>398</v>
+        <v>376</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="16" x14ac:dyDescent="0.15">
       <c r="A32" s="57" t="s">
-        <v>399</v>
+        <v>377</v>
       </c>
       <c r="B32" s="56"/>
       <c r="C32" s="56"/>
@@ -16953,7 +16751,7 @@
     </row>
     <row r="33" spans="1:8" ht="32" x14ac:dyDescent="0.15">
       <c r="A33" s="57" t="s">
-        <v>400</v>
+        <v>378</v>
       </c>
       <c r="B33" s="56"/>
       <c r="C33" s="56"/>
@@ -16965,7 +16763,7 @@
     </row>
     <row r="34" spans="1:8" ht="16" x14ac:dyDescent="0.15">
       <c r="A34" s="57" t="s">
-        <v>401</v>
+        <v>379</v>
       </c>
       <c r="B34" s="56"/>
       <c r="C34" s="56"/>
@@ -16977,7 +16775,7 @@
     </row>
     <row r="35" spans="1:8" ht="32" x14ac:dyDescent="0.15">
       <c r="A35" s="57" t="s">
-        <v>402</v>
+        <v>380</v>
       </c>
       <c r="B35" s="56"/>
       <c r="C35" s="56"/>
@@ -16989,7 +16787,7 @@
     </row>
     <row r="36" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="75" t="s">
-        <v>408</v>
+        <v>386</v>
       </c>
       <c r="B36" s="56"/>
       <c r="C36" s="56"/>
@@ -17002,7 +16800,7 @@
     <row r="37" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="60"/>
       <c r="B37" s="103" t="s">
-        <v>403</v>
+        <v>381</v>
       </c>
       <c r="C37" s="104"/>
       <c r="D37" s="104"/>
@@ -17014,11 +16812,11 @@
     <row r="38" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A38" s="60"/>
       <c r="B38" s="106" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="C38" s="107"/>
       <c r="D38" s="110" t="s">
-        <v>404</v>
+        <v>382</v>
       </c>
       <c r="E38" s="110"/>
       <c r="F38" s="110"/>
@@ -17040,41 +16838,41 @@
       <c r="B40" s="108"/>
       <c r="C40" s="109"/>
       <c r="D40" s="61" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E40" s="62" t="s">
         <v>26</v>
       </c>
       <c r="F40" s="62" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="G40" s="62" t="s">
         <v>17</v>
       </c>
       <c r="H40" s="63" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A41" s="60"/>
       <c r="B41" s="99" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="C41" s="100"/>
       <c r="D41" s="64" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E41" s="65" t="s">
         <v>26</v>
       </c>
       <c r="F41" s="66" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="G41" s="67" t="s">
         <v>17</v>
       </c>
       <c r="H41" s="68" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="15" x14ac:dyDescent="0.2">
@@ -17084,38 +16882,38 @@
       </c>
       <c r="C42" s="100"/>
       <c r="D42" s="64" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E42" s="65" t="s">
         <v>26</v>
       </c>
       <c r="F42" s="66" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="G42" s="67" t="s">
         <v>17</v>
       </c>
       <c r="H42" s="68" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A43" s="60"/>
       <c r="B43" s="99" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="C43" s="100"/>
       <c r="D43" s="64" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E43" s="65" t="s">
         <v>26</v>
       </c>
       <c r="F43" s="66" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="G43" s="66" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="H43" s="69" t="s">
         <v>17</v>
@@ -17128,7 +16926,7 @@
       </c>
       <c r="C44" s="100"/>
       <c r="D44" s="64" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E44" s="65" t="s">
         <v>26</v>
@@ -17140,20 +16938,20 @@
         <v>26</v>
       </c>
       <c r="H44" s="70" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A45" s="60"/>
       <c r="B45" s="101" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C45" s="102"/>
       <c r="D45" s="71" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E45" s="71" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="F45" s="72" t="s">
         <v>26</v>
@@ -17187,7 +16985,7 @@
     </row>
     <row r="48" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B48" s="114" t="s">
-        <v>405</v>
+        <v>383</v>
       </c>
       <c r="C48" s="115"/>
       <c r="D48" s="115"/>
@@ -17198,11 +16996,11 @@
     </row>
     <row r="49" spans="2:8" x14ac:dyDescent="0.15">
       <c r="B49" s="106" t="s">
-        <v>406</v>
+        <v>384</v>
       </c>
       <c r="C49" s="107"/>
       <c r="D49" s="110" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="E49" s="110"/>
       <c r="F49" s="110"/>
@@ -17222,40 +17020,40 @@
       <c r="B51" s="108"/>
       <c r="C51" s="109"/>
       <c r="D51" s="61" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E51" s="62" t="s">
         <v>26</v>
       </c>
       <c r="F51" s="62" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="G51" s="62" t="s">
         <v>17</v>
       </c>
       <c r="H51" s="63" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
     </row>
     <row r="52" spans="2:8" x14ac:dyDescent="0.15">
       <c r="B52" s="99" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="C52" s="100"/>
       <c r="D52" s="64" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E52" s="65" t="s">
         <v>26</v>
       </c>
       <c r="F52" s="66" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="G52" s="67" t="s">
         <v>17</v>
       </c>
       <c r="H52" s="68" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
     </row>
     <row r="53" spans="2:8" x14ac:dyDescent="0.15">
@@ -17264,37 +17062,37 @@
       </c>
       <c r="C53" s="100"/>
       <c r="D53" s="64" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E53" s="65" t="s">
         <v>26</v>
       </c>
       <c r="F53" s="66" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="G53" s="67" t="s">
         <v>17</v>
       </c>
       <c r="H53" s="68" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
     </row>
     <row r="54" spans="2:8" x14ac:dyDescent="0.15">
       <c r="B54" s="99" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="C54" s="100"/>
       <c r="D54" s="64" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E54" s="65" t="s">
         <v>26</v>
       </c>
       <c r="F54" s="66" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="G54" s="66" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="H54" s="69" t="s">
         <v>17</v>
@@ -17306,7 +17104,7 @@
       </c>
       <c r="C55" s="100"/>
       <c r="D55" s="64" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E55" s="65" t="s">
         <v>26</v>
@@ -17318,19 +17116,19 @@
         <v>26</v>
       </c>
       <c r="H55" s="70" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
     </row>
     <row r="56" spans="2:8" ht="14" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B56" s="101" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C56" s="102"/>
       <c r="D56" s="71" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E56" s="71" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="F56" s="72" t="s">
         <v>26</v>

</xml_diff>